<commit_message>
cells now properly contain types, instead of all treated as strings
</commit_message>
<xml_diff>
--- a/lib/excel/example.xlsx
+++ b/lib/excel/example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,12 +22,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t xml:space="preserve">hello</t>
   </si>
   <si>
     <t xml:space="preserve">I am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test3</t>
   </si>
   <si>
     <t xml:space="preserve">I</t>
@@ -127,14 +136,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="D4:G8"/>
+  <dimension ref="D3:J8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="C6:E7 D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="0" t="e">
+        <f aca="false">0/0</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -165,7 +180,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="n">
-        <v>1</v>
+        <v>6E-006</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
@@ -179,7 +194,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="0" t="n">
-        <v>2</v>
+        <v>2.2</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>2</v>
@@ -224,10 +239,10 @@
   <dimension ref="D12:G14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="1" sqref="C6:E7 B14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
@@ -287,14 +302,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="C4:E7"/>
+  <dimension ref="C3:E7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6:E7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="n">
         <v>1</v>
@@ -312,7 +338,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="0" t="str">
         <f aca="false">C5&amp;D5</f>
@@ -336,7 +362,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E7" s="0" t="str">
         <f aca="false">C7&amp;D7</f>

</xml_diff>